<commit_message>
Published state of ETDataset on 11 October 2017
</commit_message>
<xml_diff>
--- a/nodes_source_analyses/households/households_space_heater_heatpump_ground_water_electricity.converter.xlsx
+++ b/nodes_source_analyses/households/households_space_heater_heatpump_ground_water_electricity.converter.xlsx
@@ -1,19 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27907"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dorinevandervlies/Projects/etdataset/nodes_source_analyses/households/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="23460" tabRatio="762" activeTab="1"/>
+    <workbookView xWindow="13960" yWindow="460" windowWidth="13960" windowHeight="17540" tabRatio="762" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="14" r:id="rId1"/>
     <sheet name="Dashboard" sheetId="12" r:id="rId2"/>
     <sheet name="Research data" sheetId="13" r:id="rId3"/>
     <sheet name="Sources" sheetId="15" r:id="rId4"/>
+    <sheet name="Notes" sheetId="16" r:id="rId5"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
   <definedNames>
     <definedName name="exchange_rate_2011_2010">#REF!</definedName>
@@ -30,8 +36,11 @@
     <definedName name="Wp_to_kWp">#REF!</definedName>
     <definedName name="WP_to_MWp">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="140001" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -40,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="163">
   <si>
     <t>Source</t>
   </si>
@@ -348,31 +357,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>K</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>We</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>euro/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>KW</t>
     </r>
     <r>
@@ -492,16 +476,159 @@
   <si>
     <t>ETM Library URL</t>
   </si>
+  <si>
+    <t>Quintel WD</t>
+  </si>
+  <si>
+    <t>DHPA</t>
+  </si>
+  <si>
+    <t>NL</t>
+  </si>
+  <si>
+    <t>Phone conversation Peter Wagener notes:</t>
+  </si>
+  <si>
+    <t>201707_Tabel RV WW en koude met warmtepompen</t>
+  </si>
+  <si>
+    <t>0 until more information from DHPA is available</t>
+  </si>
+  <si>
+    <t>storage.volume</t>
+  </si>
+  <si>
+    <t>MWh</t>
+  </si>
+  <si>
+    <t>storage.cost_per_mwh</t>
+  </si>
+  <si>
+    <t>euro/MWh</t>
+  </si>
+  <si>
+    <t>ISSO 72 and Quintel calc</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>https://warmtepomp-weetjes.nl/warmtepomp/buffervat/</t>
+  </si>
+  <si>
+    <t>Warmtepompforum</t>
+  </si>
+  <si>
+    <t>http://www.warmtepompforum.nl/Volumebuffervat.php</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>buffer time</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>output capacity</t>
+  </si>
+  <si>
+    <t>kW output</t>
+  </si>
+  <si>
+    <t>specific capacity water</t>
+  </si>
+  <si>
+    <t>kJ/oC/l</t>
+  </si>
+  <si>
+    <t>temperature difference system</t>
+  </si>
+  <si>
+    <t>oC</t>
+  </si>
+  <si>
+    <t>Educated guess based on various sources</t>
+  </si>
+  <si>
+    <t>volume of buffer</t>
+  </si>
+  <si>
+    <t>liter</t>
+  </si>
+  <si>
+    <t>conversion kJ to kWh</t>
+  </si>
+  <si>
+    <t>kJ to kWh</t>
+  </si>
+  <si>
+    <t>Hot water boiler vessel used as storage device to protect compressor</t>
+  </si>
+  <si>
+    <t>delta T</t>
+  </si>
+  <si>
+    <t>specific heat capacity of water</t>
+  </si>
+  <si>
+    <t>kJ/l</t>
+  </si>
+  <si>
+    <t>kJ/MWh</t>
+  </si>
+  <si>
+    <t>MWh/liter</t>
+  </si>
+  <si>
+    <t>euro/liter</t>
+  </si>
+  <si>
+    <t>https://www.installand.nl/shop/verwarming/warmtepomp/nibe-buffervat-ukv-500-80302</t>
+  </si>
+  <si>
+    <t>Installand</t>
+  </si>
+  <si>
+    <t>costs including VAT</t>
+  </si>
+  <si>
+    <t>costs excluding VAT</t>
+  </si>
+  <si>
+    <t>costs/liter</t>
+  </si>
+  <si>
+    <t>Nefit</t>
+  </si>
+  <si>
+    <t>http://nl.documents2.nefit.nl/download/pdf/file/6720819095.pdf</t>
+  </si>
+  <si>
+    <t>Initial investment (including boiler)</t>
+  </si>
+  <si>
+    <t>Costs for boiler</t>
+  </si>
+  <si>
+    <t>See documentation Households water heater heatpump ground water electricity</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="170" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -697,6 +824,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Lettertype hoofdtekst"/>
     </font>
   </fonts>
   <fills count="13">
@@ -1265,7 +1398,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="141">
+  <cellXfs count="193">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1397,9 +1530,6 @@
     <xf numFmtId="3" fontId="12" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1469,6 +1599,55 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="12" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="12" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1496,7 +1675,33 @@
     <xf numFmtId="0" fontId="27" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="12" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="12" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="25" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="177" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="25" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="255">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1757,6 +1962,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1792,7 +2002,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1800,6 +2010,12 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
           </xdr:spPr>
           <xdr:txBody>
             <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
@@ -1830,8 +2046,203 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>886125</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>19538</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>10686733</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>105449</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13573425" y="4502638"/>
+          <a:ext cx="10753108" cy="1914711"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>937845</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>97691</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>6459758</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>172397</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13625145" y="6612791"/>
+          <a:ext cx="6474413" cy="2716306"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>887307</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>64347</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>5262880</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>1193</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13577147" y="6373707"/>
+          <a:ext cx="5330613" cy="2781646"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>10591800</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13644880" y="9560560"/>
+          <a:ext cx="10591800" cy="1117600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>111760</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>162560</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>11033760</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>162560</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13756640" y="10739120"/>
+          <a:ext cx="10922000" cy="406400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Cover Sheet"/>
@@ -2270,50 +2681,50 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.375" style="26" customWidth="1"/>
-    <col min="2" max="2" width="9.125" style="18" customWidth="1"/>
-    <col min="3" max="3" width="48.75" style="18" customWidth="1"/>
-    <col min="4" max="16384" width="10.625" style="18"/>
+    <col min="1" max="1" width="3.42578125" style="26" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="18" customWidth="1"/>
+    <col min="3" max="3" width="48.7109375" style="18" customWidth="1"/>
+    <col min="4" max="16384" width="10.7109375" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="24" customFormat="1">
+    <row r="1" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="22"/>
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
     </row>
-    <row r="2" spans="1:3" ht="20">
+    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="25" t="s">
         <v>16</v>
       </c>
       <c r="C2" s="25"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="4" t="s">
         <v>70</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="6" t="s">
         <v>19</v>
@@ -2322,128 +2733,123 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
-      <c r="B9" s="85" t="s">
+      <c r="B9" s="84" t="s">
         <v>71</v>
       </c>
-      <c r="C9" s="86"/>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="C9" s="85"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
-      <c r="B10" s="87"/>
-      <c r="C10" s="88"/>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="B10" s="86"/>
+      <c r="C10" s="87"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
-      <c r="B11" s="87" t="s">
+      <c r="B11" s="86" t="s">
         <v>72</v>
       </c>
-      <c r="C11" s="89" t="s">
+      <c r="C11" s="88" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="16" thickBot="1">
+    <row r="12" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="87"/>
+      <c r="B12" s="86"/>
       <c r="C12" s="14" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="16" thickBot="1">
+    <row r="13" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="87"/>
-      <c r="C13" s="90" t="s">
+      <c r="B13" s="86"/>
+      <c r="C13" s="89" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
-      <c r="B14" s="87"/>
-      <c r="C14" s="88" t="s">
+      <c r="B14" s="86"/>
+      <c r="C14" s="87" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
-      <c r="B15" s="87"/>
-      <c r="C15" s="88"/>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="B15" s="86"/>
+      <c r="C15" s="87"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
-      <c r="B16" s="87" t="s">
+      <c r="B16" s="86" t="s">
         <v>77</v>
       </c>
-      <c r="C16" s="91" t="s">
+      <c r="C16" s="90" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
-      <c r="B17" s="87"/>
-      <c r="C17" s="92" t="s">
+      <c r="B17" s="86"/>
+      <c r="C17" s="91" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
-      <c r="B18" s="87"/>
-      <c r="C18" s="93" t="s">
+      <c r="B18" s="86"/>
+      <c r="C18" s="92" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
-      <c r="B19" s="87"/>
-      <c r="C19" s="94" t="s">
+      <c r="B19" s="86"/>
+      <c r="C19" s="93" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
-      <c r="B20" s="95"/>
-      <c r="C20" s="96" t="s">
+      <c r="B20" s="94"/>
+      <c r="C20" s="95" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
-      <c r="B21" s="95"/>
-      <c r="C21" s="97" t="s">
+      <c r="B21" s="94"/>
+      <c r="C21" s="96" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
-      <c r="B22" s="95"/>
-      <c r="C22" s="98" t="s">
+      <c r="B22" s="94"/>
+      <c r="C22" s="97" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
-      <c r="B23" s="95"/>
-      <c r="C23" s="99" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B23" s="94"/>
+      <c r="C23" s="98" t="s">
         <v>85</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2452,63 +2858,63 @@
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="B1:K48"/>
+  <dimension ref="B1:K50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.25" style="34" customWidth="1"/>
-    <col min="2" max="2" width="3.75" style="34" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" style="34" customWidth="1"/>
+    <col min="2" max="2" width="3.7109375" style="34" customWidth="1"/>
     <col min="3" max="3" width="46" style="34" customWidth="1"/>
-    <col min="4" max="4" width="12.75" style="34" customWidth="1"/>
-    <col min="5" max="5" width="17.375" style="34" customWidth="1"/>
-    <col min="6" max="6" width="4.625" style="34" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="34" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" style="34" customWidth="1"/>
+    <col min="6" max="6" width="4.5703125" style="34" customWidth="1"/>
     <col min="7" max="7" width="45" style="34" customWidth="1"/>
-    <col min="8" max="8" width="5.125" style="34" customWidth="1"/>
-    <col min="9" max="9" width="46.125" style="34" customWidth="1"/>
-    <col min="10" max="10" width="5.375" style="34" customWidth="1"/>
-    <col min="11" max="16384" width="10.625" style="34"/>
+    <col min="8" max="8" width="5.140625" style="34" customWidth="1"/>
+    <col min="9" max="9" width="46.140625" style="34" customWidth="1"/>
+    <col min="10" max="10" width="5.42578125" style="34" customWidth="1"/>
+    <col min="11" max="16384" width="10.7109375" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.2">
       <c r="D1" s="32"/>
       <c r="E1" s="32"/>
       <c r="F1" s="32"/>
       <c r="G1" s="32"/>
     </row>
-    <row r="2" spans="2:11">
-      <c r="B2" s="131" t="s">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B2" s="163" t="s">
         <v>86</v>
       </c>
-      <c r="C2" s="132"/>
-      <c r="D2" s="132"/>
-      <c r="E2" s="133"/>
+      <c r="C2" s="164"/>
+      <c r="D2" s="164"/>
+      <c r="E2" s="165"/>
       <c r="F2" s="32"/>
       <c r="G2" s="32"/>
     </row>
-    <row r="3" spans="2:11">
-      <c r="B3" s="134"/>
-      <c r="C3" s="135"/>
-      <c r="D3" s="135"/>
-      <c r="E3" s="136"/>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B3" s="166"/>
+      <c r="C3" s="167"/>
+      <c r="D3" s="167"/>
+      <c r="E3" s="168"/>
       <c r="F3" s="32"/>
       <c r="G3" s="32"/>
     </row>
-    <row r="4" spans="2:11">
-      <c r="B4" s="137"/>
-      <c r="C4" s="138"/>
-      <c r="D4" s="138"/>
-      <c r="E4" s="139"/>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B4" s="169"/>
+      <c r="C4" s="170"/>
+      <c r="D4" s="170"/>
+      <c r="E4" s="171"/>
       <c r="F4" s="32"/>
       <c r="G4" s="32"/>
     </row>
-    <row r="5" spans="2:11" ht="16" thickBot="1">
+    <row r="5" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D5" s="32"/>
     </row>
-    <row r="6" spans="2:11">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B6" s="35"/>
       <c r="C6" s="16"/>
       <c r="D6" s="16"/>
@@ -2519,12 +2925,12 @@
       <c r="I6" s="16"/>
       <c r="J6" s="36"/>
     </row>
-    <row r="7" spans="2:11" s="41" customFormat="1" ht="18">
-      <c r="B7" s="100"/>
+    <row r="7" spans="2:11" s="41" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="B7" s="99"/>
       <c r="C7" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="101" t="s">
+      <c r="D7" s="100" t="s">
         <v>13</v>
       </c>
       <c r="E7" s="15" t="s">
@@ -2538,9 +2944,9 @@
       <c r="I7" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="J7" s="107"/>
-    </row>
-    <row r="8" spans="2:11" s="41" customFormat="1" ht="18">
+      <c r="J7" s="106"/>
+    </row>
+    <row r="8" spans="2:11" s="41" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="B8" s="20"/>
       <c r="C8" s="14"/>
       <c r="D8" s="28"/>
@@ -2551,10 +2957,10 @@
       <c r="I8" s="14"/>
       <c r="J8" s="42"/>
     </row>
-    <row r="9" spans="2:11" s="41" customFormat="1" ht="19" thickBot="1">
+    <row r="9" spans="2:11" s="41" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="20"/>
       <c r="C9" s="14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D9" s="28"/>
       <c r="E9" s="14"/>
@@ -2564,10 +2970,10 @@
       <c r="I9" s="14"/>
       <c r="J9" s="42"/>
     </row>
-    <row r="10" spans="2:11" s="41" customFormat="1" ht="19" thickBot="1">
+    <row r="10" spans="2:11" s="41" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="20"/>
-      <c r="C10" s="125" t="s">
-        <v>108</v>
+      <c r="C10" s="124" t="s">
+        <v>107</v>
       </c>
       <c r="D10" s="17" t="s">
         <v>4</v>
@@ -2578,15 +2984,15 @@
       <c r="F10" s="33"/>
       <c r="G10" s="33"/>
       <c r="H10" s="27"/>
-      <c r="I10" s="140" t="s">
+      <c r="I10" s="130" t="s">
         <v>52</v>
       </c>
       <c r="J10" s="42"/>
     </row>
-    <row r="11" spans="2:11" s="41" customFormat="1" ht="19" thickBot="1">
+    <row r="11" spans="2:11" s="41" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="20"/>
-      <c r="C11" s="125" t="s">
-        <v>109</v>
+      <c r="C11" s="124" t="s">
+        <v>108</v>
       </c>
       <c r="D11" s="17" t="s">
         <v>4</v>
@@ -2602,10 +3008,10 @@
       </c>
       <c r="J11" s="42"/>
     </row>
-    <row r="12" spans="2:11" s="41" customFormat="1" ht="19" thickBot="1">
+    <row r="12" spans="2:11" s="41" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="20"/>
-      <c r="C12" s="125" t="s">
-        <v>110</v>
+      <c r="C12" s="124" t="s">
+        <v>109</v>
       </c>
       <c r="D12" s="17" t="s">
         <v>4</v>
@@ -2621,55 +3027,56 @@
       </c>
       <c r="J12" s="42"/>
     </row>
-    <row r="13" spans="2:11" ht="16" thickBot="1">
-      <c r="B13" s="37"/>
-      <c r="C13" s="33" t="s">
+    <row r="13" spans="2:11" s="41" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="20"/>
+      <c r="C13" s="144" t="s">
+        <v>122</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="E13" s="162">
+        <f>'Research data'!G7</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="143"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="31" t="str">
+        <f>Sources!E13</f>
+        <v>ISSO 72 and Quintel calc</v>
+      </c>
+      <c r="J13" s="42"/>
+    </row>
+    <row r="14" spans="2:11" s="41" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="20"/>
+      <c r="C14" s="144" t="s">
+        <v>124</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="E14" s="145">
+        <f>'Research data'!G8</f>
+        <v>154736.84210526317</v>
+      </c>
+      <c r="F14" s="143"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="130" t="s">
+        <v>116</v>
+      </c>
+      <c r="J14" s="42"/>
+    </row>
+    <row r="15" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="37"/>
+      <c r="C15" s="33" t="s">
         <v>32</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E13" s="43">
-        <v>0</v>
-      </c>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="J13" s="108"/>
-      <c r="K13" s="32"/>
-    </row>
-    <row r="14" spans="2:11" ht="16" thickBot="1">
-      <c r="B14" s="37"/>
-      <c r="C14" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E14" s="44">
-        <v>0</v>
-      </c>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="J14" s="108"/>
-      <c r="K14" s="32"/>
-    </row>
-    <row r="15" spans="2:11" ht="16" thickBot="1">
-      <c r="B15" s="37"/>
-      <c r="C15" s="125" t="s">
-        <v>111</v>
       </c>
       <c r="D15" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="44">
+      <c r="E15" s="43">
         <v>0</v>
       </c>
       <c r="F15" s="33"/>
@@ -2678,19 +3085,19 @@
       <c r="I15" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="J15" s="108"/>
+      <c r="J15" s="107"/>
       <c r="K15" s="32"/>
     </row>
-    <row r="16" spans="2:11" ht="16" thickBot="1">
+    <row r="16" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="37"/>
       <c r="C16" s="33" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="D16" s="19" t="s">
         <v>4</v>
       </c>
       <c r="E16" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" s="33"/>
       <c r="G16" s="33"/>
@@ -2698,18 +3105,18 @@
       <c r="I16" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="J16" s="108"/>
+      <c r="J16" s="107"/>
       <c r="K16" s="32"/>
     </row>
-    <row r="17" spans="2:11" ht="16" thickBot="1">
+    <row r="17" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="37"/>
-      <c r="C17" s="33" t="s">
-        <v>37</v>
+      <c r="C17" s="124" t="s">
+        <v>110</v>
       </c>
       <c r="D17" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E17" s="31">
+      <c r="E17" s="44">
         <v>0</v>
       </c>
       <c r="F17" s="33"/>
@@ -2718,19 +3125,19 @@
       <c r="I17" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="J17" s="108"/>
+      <c r="J17" s="107"/>
       <c r="K17" s="32"/>
     </row>
-    <row r="18" spans="2:11" ht="16" thickBot="1">
+    <row r="18" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="37"/>
       <c r="C18" s="33" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="D18" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="31">
-        <v>0</v>
+      <c r="E18" s="44">
+        <v>1</v>
       </c>
       <c r="F18" s="33"/>
       <c r="G18" s="33"/>
@@ -2738,249 +3145,247 @@
       <c r="I18" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="J18" s="108"/>
+      <c r="J18" s="107"/>
       <c r="K18" s="32"/>
     </row>
-    <row r="19" spans="2:11" ht="16" thickBot="1">
+    <row r="19" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="37"/>
       <c r="C19" s="33" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="E19" s="44">
+        <v>4</v>
+      </c>
+      <c r="E19" s="31">
         <v>0</v>
       </c>
       <c r="F19" s="33"/>
-      <c r="G19" s="33" t="s">
-        <v>27</v>
-      </c>
+      <c r="G19" s="33"/>
       <c r="H19" s="33"/>
       <c r="I19" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="J19" s="108"/>
-    </row>
-    <row r="20" spans="2:11" ht="16" thickBot="1">
+      <c r="J19" s="107"/>
+      <c r="K19" s="32"/>
+    </row>
+    <row r="20" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="37"/>
       <c r="C20" s="33" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="E20" s="43">
-        <f>'Research data'!G6</f>
-        <v>0.01</v>
+        <v>4</v>
+      </c>
+      <c r="E20" s="31">
+        <v>0</v>
       </c>
       <c r="F20" s="33"/>
-      <c r="G20" s="33" t="s">
-        <v>53</v>
-      </c>
+      <c r="G20" s="33"/>
       <c r="H20" s="33"/>
       <c r="I20" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="J20" s="108"/>
-    </row>
-    <row r="21" spans="2:11" ht="16" thickBot="1">
+      <c r="J20" s="107"/>
+      <c r="K20" s="32"/>
+    </row>
+    <row r="21" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B21" s="37"/>
-      <c r="C21" s="59" t="s">
-        <v>60</v>
+      <c r="C21" s="33" t="s">
+        <v>39</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E21" s="43">
-        <v>1.9574835417698999</v>
+        <v>59</v>
+      </c>
+      <c r="E21" s="44">
+        <v>0</v>
       </c>
       <c r="F21" s="33"/>
-      <c r="G21" s="60" t="s">
-        <v>65</v>
+      <c r="G21" s="33" t="s">
+        <v>27</v>
       </c>
       <c r="H21" s="33"/>
       <c r="I21" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="J21" s="108"/>
-    </row>
-    <row r="22" spans="2:11" ht="16" thickBot="1">
+      <c r="J21" s="107"/>
+    </row>
+    <row r="22" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B22" s="37"/>
-      <c r="C22" s="59" t="s">
-        <v>61</v>
+      <c r="C22" s="33" t="s">
+        <v>40</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>4</v>
+        <v>59</v>
       </c>
       <c r="E22" s="43">
-        <v>0.48469874776884098</v>
+        <f>'Research data'!G6</f>
+        <v>0.01</v>
       </c>
       <c r="F22" s="33"/>
-      <c r="G22" s="60" t="s">
-        <v>66</v>
+      <c r="G22" s="33" t="s">
+        <v>53</v>
       </c>
       <c r="H22" s="33"/>
       <c r="I22" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="J22" s="108"/>
-    </row>
-    <row r="23" spans="2:11" ht="16" thickBot="1">
+      <c r="J22" s="107"/>
+    </row>
+    <row r="23" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B23" s="37"/>
       <c r="C23" s="59" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D23" s="19" t="s">
         <v>4</v>
       </c>
       <c r="E23" s="43">
-        <v>2.80578502945801</v>
+        <v>1.9574835417698999</v>
       </c>
       <c r="F23" s="33"/>
       <c r="G23" s="60" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H23" s="33"/>
       <c r="I23" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="J23" s="108"/>
-    </row>
-    <row r="24" spans="2:11" ht="16" thickBot="1">
+      <c r="J23" s="107"/>
+    </row>
+    <row r="24" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="37"/>
       <c r="C24" s="59" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D24" s="19" t="s">
         <v>4</v>
       </c>
       <c r="E24" s="43">
-        <v>3.66713847099266</v>
+        <v>0.48469874776884098</v>
       </c>
       <c r="F24" s="33"/>
       <c r="G24" s="60" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H24" s="33"/>
       <c r="I24" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="J24" s="108"/>
-    </row>
-    <row r="25" spans="2:11" ht="16" thickBot="1">
+      <c r="J24" s="107"/>
+    </row>
+    <row r="25" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B25" s="37"/>
       <c r="C25" s="59" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D25" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E25" s="44">
+      <c r="E25" s="43">
+        <v>2.80578502945801</v>
+      </c>
+      <c r="F25" s="33"/>
+      <c r="G25" s="60" t="s">
+        <v>67</v>
+      </c>
+      <c r="H25" s="33"/>
+      <c r="I25" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="J25" s="107"/>
+    </row>
+    <row r="26" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="37"/>
+      <c r="C26" s="59" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" s="43">
+        <v>3.66713847099266</v>
+      </c>
+      <c r="F26" s="33"/>
+      <c r="G26" s="60" t="s">
+        <v>68</v>
+      </c>
+      <c r="H26" s="33"/>
+      <c r="I26" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="J26" s="107"/>
+    </row>
+    <row r="27" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="37"/>
+      <c r="C27" s="59" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="44">
         <v>5524.9193295064797</v>
       </c>
-      <c r="F25" s="33"/>
-      <c r="G25" s="61" t="s">
+      <c r="F27" s="33"/>
+      <c r="G27" s="61" t="s">
         <v>69</v>
       </c>
-      <c r="H25" s="33"/>
-      <c r="I25" s="126" t="s">
+      <c r="H27" s="33"/>
+      <c r="I27" s="125" t="s">
         <v>52</v>
       </c>
-      <c r="J25" s="108"/>
-    </row>
-    <row r="26" spans="2:11">
-      <c r="B26" s="37"/>
-      <c r="C26" s="76"/>
-      <c r="D26" s="103"/>
-      <c r="E26" s="104"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="76"/>
-      <c r="H26" s="32"/>
-      <c r="I26" s="32"/>
-      <c r="J26" s="108"/>
-    </row>
-    <row r="27" spans="2:11" ht="16" thickBot="1">
-      <c r="B27" s="37"/>
-      <c r="C27" s="14" t="s">
+      <c r="J27" s="107"/>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B28" s="37"/>
+      <c r="C28" s="76"/>
+      <c r="D28" s="102"/>
+      <c r="E28" s="103"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="76"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="107"/>
+    </row>
+    <row r="29" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="37"/>
+      <c r="C29" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="D27" s="103"/>
-      <c r="E27" s="104"/>
-      <c r="F27" s="32"/>
-      <c r="G27" s="76"/>
-      <c r="H27" s="32"/>
-      <c r="I27" s="32"/>
-      <c r="J27" s="108"/>
-    </row>
-    <row r="28" spans="2:11" ht="16" thickBot="1">
-      <c r="B28" s="37"/>
-      <c r="C28" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="D28" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="E28" s="44">
-        <f>'Research data'!G14</f>
-        <v>13000</v>
-      </c>
-      <c r="F28" s="33"/>
-      <c r="G28" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="H28" s="33"/>
-      <c r="I28" s="84" t="s">
-        <v>52</v>
-      </c>
-      <c r="J28" s="108"/>
-    </row>
-    <row r="29" spans="2:11" ht="16" thickBot="1">
-      <c r="B29" s="37"/>
-      <c r="C29" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="D29" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="E29" s="44">
-        <v>0</v>
-      </c>
-      <c r="F29" s="33"/>
-      <c r="G29" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="H29" s="33"/>
-      <c r="I29" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="J29" s="108"/>
-    </row>
-    <row r="30" spans="2:11" ht="16" thickBot="1">
+      <c r="D29" s="102"/>
+      <c r="E29" s="103"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="76"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="32"/>
+      <c r="J29" s="107"/>
+    </row>
+    <row r="30" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B30" s="37"/>
       <c r="C30" s="33" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D30" s="19" t="s">
         <v>31</v>
       </c>
       <c r="E30" s="44">
-        <v>0</v>
+        <f>'Research data'!G16</f>
+        <v>12746.4</v>
       </c>
       <c r="F30" s="33"/>
       <c r="G30" s="33" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="H30" s="33"/>
-      <c r="I30" s="31" t="s">
+      <c r="I30" s="83" t="s">
         <v>52</v>
       </c>
-      <c r="J30" s="108"/>
-    </row>
-    <row r="31" spans="2:11" ht="16" thickBot="1">
+      <c r="J30" s="107"/>
+    </row>
+    <row r="31" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B31" s="37"/>
       <c r="C31" s="33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D31" s="19" t="s">
         <v>31</v>
@@ -2990,270 +3395,281 @@
       </c>
       <c r="F31" s="33"/>
       <c r="G31" s="33" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="H31" s="33"/>
       <c r="I31" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="J31" s="108"/>
-    </row>
-    <row r="32" spans="2:11" ht="16" thickBot="1">
+      <c r="J31" s="107"/>
+    </row>
+    <row r="32" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B32" s="37"/>
       <c r="C32" s="33" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="E32" s="102">
-        <f>'Research data'!G16</f>
-        <v>100</v>
+        <v>31</v>
+      </c>
+      <c r="E32" s="44">
+        <f>'Research data'!G22</f>
+        <v>1500</v>
       </c>
       <c r="F32" s="33"/>
       <c r="G32" s="33" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="H32" s="33"/>
-      <c r="I32" s="84" t="s">
-        <v>52</v>
-      </c>
-      <c r="J32" s="108"/>
-    </row>
-    <row r="33" spans="2:10" ht="16" thickBot="1">
+      <c r="I32" s="83" t="str">
+        <f>Sources!E10</f>
+        <v>DHPA</v>
+      </c>
+      <c r="J32" s="107"/>
+    </row>
+    <row r="33" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B33" s="37"/>
       <c r="C33" s="33" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D33" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="E33" s="43">
-        <f>'Research data'!G18</f>
+        <v>31</v>
+      </c>
+      <c r="E33" s="44">
         <v>0</v>
       </c>
       <c r="F33" s="33"/>
       <c r="G33" s="33" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="H33" s="33"/>
-      <c r="I33" s="84" t="s">
+      <c r="I33" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="J33" s="108"/>
-    </row>
-    <row r="34" spans="2:10" ht="16" thickBot="1">
+      <c r="J33" s="107"/>
+    </row>
+    <row r="34" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B34" s="37"/>
       <c r="C34" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D34" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="E34" s="105">
-        <v>0</v>
+        <v>51</v>
+      </c>
+      <c r="E34" s="101">
+        <f>'Research data'!G18</f>
+        <v>100</v>
       </c>
       <c r="F34" s="33"/>
       <c r="G34" s="33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H34" s="33"/>
-      <c r="I34" s="115" t="s">
-        <v>52</v>
-      </c>
-      <c r="J34" s="108"/>
-    </row>
-    <row r="35" spans="2:10" ht="16" thickBot="1">
+      <c r="I34" s="83" t="str">
+        <f>Sources!E10</f>
+        <v>DHPA</v>
+      </c>
+      <c r="J34" s="107"/>
+    </row>
+    <row r="35" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B35" s="37"/>
       <c r="C35" s="33" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D35" s="19" t="s">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="E35" s="43">
-        <v>0.04</v>
+        <f>'Research data'!G20</f>
+        <v>0</v>
       </c>
       <c r="F35" s="33"/>
       <c r="G35" s="33" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="H35" s="33"/>
-      <c r="I35" s="31" t="s">
+      <c r="I35" s="83" t="s">
         <v>52</v>
       </c>
-      <c r="J35" s="108"/>
-    </row>
-    <row r="36" spans="2:10" ht="16" thickBot="1">
+      <c r="J35" s="107"/>
+    </row>
+    <row r="36" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B36" s="37"/>
       <c r="C36" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="D36" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E36" s="104">
+        <v>0</v>
+      </c>
+      <c r="F36" s="33"/>
+      <c r="G36" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="H36" s="33"/>
+      <c r="I36" s="114" t="s">
+        <v>52</v>
+      </c>
+      <c r="J36" s="107"/>
+    </row>
+    <row r="37" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="37"/>
+      <c r="C37" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="D37" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="E37" s="43">
+        <v>0.04</v>
+      </c>
+      <c r="F37" s="33"/>
+      <c r="G37" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="H37" s="33"/>
+      <c r="I37" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="J37" s="107"/>
+    </row>
+    <row r="38" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="37"/>
+      <c r="C38" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="D36" s="19" t="s">
+      <c r="D38" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="E36" s="44">
+      <c r="E38" s="44">
         <v>0</v>
       </c>
-      <c r="F36" s="33"/>
-      <c r="G36" s="33"/>
-      <c r="H36" s="33"/>
-      <c r="I36" s="31" t="s">
+      <c r="F38" s="33"/>
+      <c r="G38" s="33"/>
+      <c r="H38" s="33"/>
+      <c r="I38" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="J36" s="108"/>
-    </row>
-    <row r="37" spans="2:10">
-      <c r="B37" s="37"/>
-      <c r="C37" s="33"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="106"/>
-      <c r="F37" s="33"/>
-      <c r="G37" s="33"/>
-      <c r="H37" s="33"/>
-      <c r="I37" s="32"/>
-      <c r="J37" s="108"/>
-    </row>
-    <row r="38" spans="2:10" ht="16" thickBot="1">
-      <c r="B38" s="37"/>
-      <c r="C38" s="14" t="s">
+      <c r="J38" s="107"/>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B39" s="37"/>
+      <c r="C39" s="33"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="105"/>
+      <c r="F39" s="33"/>
+      <c r="G39" s="33"/>
+      <c r="H39" s="33"/>
+      <c r="I39" s="32"/>
+      <c r="J39" s="107"/>
+    </row>
+    <row r="40" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="37"/>
+      <c r="C40" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="D38" s="103"/>
-      <c r="E38" s="106"/>
-      <c r="F38" s="32"/>
-      <c r="G38" s="32"/>
-      <c r="H38" s="32"/>
-      <c r="I38" s="32"/>
-      <c r="J38" s="108"/>
-    </row>
-    <row r="39" spans="2:10" ht="16" thickBot="1">
-      <c r="B39" s="37"/>
-      <c r="C39" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="D39" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="E39" s="44">
-        <f>'Research data'!G9</f>
-        <v>0</v>
-      </c>
-      <c r="F39" s="33"/>
-      <c r="G39" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="H39" s="33"/>
-      <c r="I39" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="J39" s="108"/>
-    </row>
-    <row r="40" spans="2:10" ht="16" thickBot="1">
-      <c r="B40" s="37"/>
-      <c r="C40" s="130" t="s">
-        <v>47</v>
-      </c>
-      <c r="D40" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="E40" s="102">
-        <f>'Research data'!G10</f>
-        <v>0</v>
-      </c>
-      <c r="F40" s="33"/>
-      <c r="G40" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="H40" s="33"/>
-      <c r="I40" s="117" t="s">
-        <v>52</v>
-      </c>
-      <c r="J40" s="108"/>
-    </row>
-    <row r="41" spans="2:10" ht="16" thickBot="1">
+      <c r="D40" s="102"/>
+      <c r="E40" s="105"/>
+      <c r="F40" s="32"/>
+      <c r="G40" s="32"/>
+      <c r="H40" s="32"/>
+      <c r="I40" s="32"/>
+      <c r="J40" s="107"/>
+    </row>
+    <row r="41" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B41" s="37"/>
       <c r="C41" s="33" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="D41" s="19" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E41" s="44">
         <f>'Research data'!G11</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F41" s="33"/>
       <c r="G41" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="H41" s="33"/>
+      <c r="I41" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="J41" s="107"/>
+    </row>
+    <row r="42" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="37"/>
+      <c r="C42" s="129" t="s">
+        <v>47</v>
+      </c>
+      <c r="D42" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="E42" s="101">
+        <f>'Research data'!G12</f>
+        <v>0</v>
+      </c>
+      <c r="F42" s="33"/>
+      <c r="G42" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="H42" s="33"/>
+      <c r="I42" s="116" t="s">
+        <v>52</v>
+      </c>
+      <c r="J42" s="107"/>
+    </row>
+    <row r="43" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="37"/>
+      <c r="C43" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="D43" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="E43" s="44">
+        <f>'Research data'!G13</f>
+        <v>15</v>
+      </c>
+      <c r="F43" s="33"/>
+      <c r="G43" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="H41" s="33"/>
-      <c r="I41" s="118" t="s">
+      <c r="H43" s="33"/>
+      <c r="I43" s="117" t="s">
         <v>52</v>
       </c>
-      <c r="J41" s="108"/>
-    </row>
-    <row r="42" spans="2:10" ht="16" thickBot="1">
-      <c r="B42" s="37"/>
-      <c r="C42" s="33" t="s">
+      <c r="J43" s="107"/>
+    </row>
+    <row r="44" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="37"/>
+      <c r="C44" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="D42" s="19" t="s">
+      <c r="D44" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E42" s="44">
-        <v>0</v>
-      </c>
-      <c r="F42" s="33"/>
-      <c r="G42" s="33"/>
-      <c r="H42" s="33"/>
-      <c r="I42" s="126" t="s">
-        <v>52</v>
-      </c>
-      <c r="J42" s="108"/>
-    </row>
-    <row r="43" spans="2:10" ht="16" thickBot="1">
-      <c r="B43" s="37"/>
-      <c r="C43" s="121" t="s">
-        <v>101</v>
-      </c>
-      <c r="D43" s="19"/>
-      <c r="E43" s="102">
-        <v>6</v>
-      </c>
-      <c r="F43" s="33"/>
-      <c r="G43" s="33"/>
-      <c r="H43" s="33"/>
-      <c r="I43" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="J43" s="108"/>
-    </row>
-    <row r="44" spans="2:10" ht="16" thickBot="1">
-      <c r="B44" s="37"/>
-      <c r="C44" s="121" t="s">
-        <v>102</v>
-      </c>
-      <c r="D44" s="19"/>
-      <c r="E44" s="102">
+      <c r="E44" s="44">
         <v>0</v>
       </c>
       <c r="F44" s="33"/>
       <c r="G44" s="33"/>
       <c r="H44" s="33"/>
-      <c r="I44" s="31" t="s">
+      <c r="I44" s="125" t="s">
         <v>52</v>
       </c>
-      <c r="J44" s="108"/>
-    </row>
-    <row r="45" spans="2:10" ht="16" thickBot="1">
+      <c r="J44" s="107"/>
+    </row>
+    <row r="45" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B45" s="37"/>
-      <c r="C45" s="121" t="s">
-        <v>103</v>
+      <c r="C45" s="120" t="s">
+        <v>100</v>
       </c>
       <c r="D45" s="19"/>
-      <c r="E45" s="102">
-        <v>130</v>
+      <c r="E45" s="101">
+        <v>6</v>
       </c>
       <c r="F45" s="33"/>
       <c r="G45" s="33"/>
@@ -3261,16 +3677,16 @@
       <c r="I45" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="J45" s="108"/>
-    </row>
-    <row r="46" spans="2:10" ht="16" thickBot="1">
+      <c r="J45" s="107"/>
+    </row>
+    <row r="46" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B46" s="37"/>
-      <c r="C46" s="121" t="s">
-        <v>104</v>
+      <c r="C46" s="120" t="s">
+        <v>101</v>
       </c>
       <c r="D46" s="19"/>
-      <c r="E46" s="102">
-        <v>4</v>
+      <c r="E46" s="101">
+        <v>0</v>
       </c>
       <c r="F46" s="33"/>
       <c r="G46" s="33"/>
@@ -3278,16 +3694,16 @@
       <c r="I46" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="J46" s="108"/>
-    </row>
-    <row r="47" spans="2:10" ht="16" thickBot="1">
+      <c r="J46" s="107"/>
+    </row>
+    <row r="47" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B47" s="37"/>
-      <c r="C47" s="121" t="s">
-        <v>105</v>
+      <c r="C47" s="120" t="s">
+        <v>102</v>
       </c>
       <c r="D47" s="19"/>
-      <c r="E47" s="102">
-        <v>40</v>
+      <c r="E47" s="101">
+        <v>130</v>
       </c>
       <c r="F47" s="33"/>
       <c r="G47" s="33"/>
@@ -3295,18 +3711,52 @@
       <c r="I47" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="J47" s="108"/>
-    </row>
-    <row r="48" spans="2:10" ht="20" customHeight="1" thickBot="1">
-      <c r="B48" s="38"/>
-      <c r="C48" s="39"/>
-      <c r="D48" s="39"/>
-      <c r="E48" s="39"/>
-      <c r="F48" s="39"/>
-      <c r="G48" s="39"/>
-      <c r="H48" s="39"/>
-      <c r="I48" s="39"/>
-      <c r="J48" s="40"/>
+      <c r="J47" s="107"/>
+    </row>
+    <row r="48" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="37"/>
+      <c r="C48" s="120" t="s">
+        <v>103</v>
+      </c>
+      <c r="D48" s="19"/>
+      <c r="E48" s="101">
+        <v>4</v>
+      </c>
+      <c r="F48" s="33"/>
+      <c r="G48" s="33"/>
+      <c r="H48" s="33"/>
+      <c r="I48" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="J48" s="107"/>
+    </row>
+    <row r="49" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="37"/>
+      <c r="C49" s="120" t="s">
+        <v>104</v>
+      </c>
+      <c r="D49" s="19"/>
+      <c r="E49" s="101">
+        <v>40</v>
+      </c>
+      <c r="F49" s="33"/>
+      <c r="G49" s="33"/>
+      <c r="H49" s="33"/>
+      <c r="I49" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="J49" s="107"/>
+    </row>
+    <row r="50" spans="2:10" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="38"/>
+      <c r="C50" s="39"/>
+      <c r="D50" s="39"/>
+      <c r="E50" s="39"/>
+      <c r="F50" s="39"/>
+      <c r="G50" s="39"/>
+      <c r="H50" s="39"/>
+      <c r="I50" s="39"/>
+      <c r="J50" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3346,11 +3796,6 @@
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3359,30 +3804,30 @@
   <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0">
     <tabColor theme="6" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="B1:K19"/>
+  <dimension ref="B1:O22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.375" style="62" customWidth="1"/>
-    <col min="2" max="2" width="3.5" style="62" customWidth="1"/>
-    <col min="3" max="3" width="35.875" style="62" customWidth="1"/>
-    <col min="4" max="4" width="16.625" style="62" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="13.875" style="62" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="12.625" style="62" customWidth="1"/>
-    <col min="7" max="7" width="10.75" style="62" customWidth="1"/>
-    <col min="8" max="8" width="4" style="62" customWidth="1"/>
-    <col min="9" max="9" width="16" style="62" customWidth="1"/>
-    <col min="10" max="10" width="3" style="63" customWidth="1"/>
-    <col min="11" max="11" width="60" style="62" customWidth="1"/>
-    <col min="12" max="16384" width="10.625" style="62"/>
+    <col min="1" max="2" width="3.42578125" style="62" customWidth="1"/>
+    <col min="3" max="3" width="35.85546875" style="62" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" style="62" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="62" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" style="62" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" style="62" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.5703125" style="62" customWidth="1"/>
+    <col min="9" max="10" width="8.5703125" style="62" customWidth="1"/>
+    <col min="11" max="13" width="16" style="62" customWidth="1"/>
+    <col min="14" max="14" width="3" style="63" customWidth="1"/>
+    <col min="15" max="15" width="60" style="62" customWidth="1"/>
+    <col min="16" max="16384" width="10.7109375" style="62"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="16" thickBot="1"/>
-    <row r="2" spans="2:11">
+    <row r="1" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B2" s="64"/>
       <c r="C2" s="65"/>
       <c r="D2" s="65"/>
@@ -3391,30 +3836,52 @@
       <c r="G2" s="65"/>
       <c r="H2" s="65"/>
       <c r="I2" s="65"/>
-      <c r="J2" s="66"/>
+      <c r="J2" s="65"/>
       <c r="K2" s="65"/>
-    </row>
-    <row r="3" spans="2:11" s="21" customFormat="1">
+      <c r="L2" s="65"/>
+      <c r="M2" s="65"/>
+      <c r="N2" s="66"/>
+      <c r="O2" s="65"/>
+    </row>
+    <row r="3" spans="2:15" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="20"/>
-      <c r="C3" s="113" t="s">
+      <c r="C3" s="112" t="s">
         <v>89</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="113" t="s">
+      <c r="F3" s="112" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="113" t="s">
+      <c r="G3" s="112" t="s">
         <v>82</v>
       </c>
-      <c r="H3" s="113"/>
-      <c r="I3" s="113"/>
-      <c r="J3" s="58"/>
-      <c r="K3" s="113" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11">
+      <c r="H3" s="112"/>
+      <c r="I3" s="112" t="s">
+        <v>117</v>
+      </c>
+      <c r="J3" s="112" t="str">
+        <f>Sources!E13</f>
+        <v>ISSO 72 and Quintel calc</v>
+      </c>
+      <c r="K3" s="112" t="str">
+        <f>Sources!E15</f>
+        <v>Warmtepompforum</v>
+      </c>
+      <c r="L3" s="112" t="str">
+        <f>Sources!E17</f>
+        <v>Installand</v>
+      </c>
+      <c r="M3" s="112" t="str">
+        <f>Sources!E19</f>
+        <v>Nefit</v>
+      </c>
+      <c r="N3" s="58"/>
+      <c r="O3" s="112" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B4" s="67"/>
       <c r="C4" s="68"/>
       <c r="D4" s="68"/>
@@ -3423,10 +3890,14 @@
       <c r="G4" s="69"/>
       <c r="H4" s="69"/>
       <c r="I4" s="69"/>
-      <c r="J4" s="112"/>
-      <c r="K4" s="9"/>
-    </row>
-    <row r="5" spans="2:11" ht="16" thickBot="1">
+      <c r="J4" s="69"/>
+      <c r="K4" s="69"/>
+      <c r="L4" s="69"/>
+      <c r="M4" s="69"/>
+      <c r="N4" s="111"/>
+      <c r="O4" s="9"/>
+    </row>
+    <row r="5" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="67"/>
       <c r="C5" s="29" t="s">
         <v>88</v>
@@ -3438,251 +3909,390 @@
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
-      <c r="K5" s="59"/>
-    </row>
-    <row r="6" spans="2:11" ht="16" thickBot="1">
+      <c r="K5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="59"/>
+    </row>
+    <row r="6" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="67"/>
-      <c r="C6" s="127" t="s">
-        <v>112</v>
+      <c r="C6" s="126" t="s">
+        <v>111</v>
       </c>
       <c r="D6" s="70"/>
       <c r="E6" s="70"/>
       <c r="F6" s="71" t="s">
         <v>59</v>
       </c>
-      <c r="G6" s="128">
+      <c r="G6" s="127">
         <f>ROUND(0.01,2)</f>
         <v>0.01</v>
       </c>
-      <c r="H6" s="72"/>
+      <c r="H6" s="140"/>
       <c r="I6" s="72"/>
-      <c r="J6" s="69"/>
-      <c r="K6" s="59"/>
-    </row>
-    <row r="7" spans="2:11">
+      <c r="J6" s="72"/>
+      <c r="K6" s="72"/>
+      <c r="L6" s="72"/>
+      <c r="M6" s="72"/>
+      <c r="N6" s="69"/>
+      <c r="O6" s="59"/>
+    </row>
+    <row r="7" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="67"/>
-      <c r="C7" s="75"/>
-      <c r="D7" s="75"/>
-      <c r="E7" s="75"/>
-      <c r="F7" s="76"/>
-      <c r="G7" s="73"/>
-      <c r="H7" s="73"/>
-      <c r="I7" s="73"/>
-      <c r="J7" s="73"/>
-      <c r="K7" s="114"/>
-    </row>
-    <row r="8" spans="2:11" ht="16" thickBot="1">
+      <c r="C7" s="142" t="s">
+        <v>122</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="E7" s="70"/>
+      <c r="F7" s="143" t="s">
+        <v>123</v>
+      </c>
+      <c r="G7" s="161">
+        <f>I7</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="140"/>
+      <c r="I7" s="173">
+        <f>Notes!E24</f>
+        <v>0</v>
+      </c>
+      <c r="J7" s="161">
+        <f>Notes!E13</f>
+        <v>1.7000000000000001E-3</v>
+      </c>
+      <c r="K7" s="161">
+        <f>Notes!E21</f>
+        <v>3.3E-3</v>
+      </c>
+      <c r="L7" s="179"/>
+      <c r="M7" s="179"/>
+      <c r="N7" s="69"/>
+      <c r="O7" s="133"/>
+    </row>
+    <row r="8" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="67"/>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="142" t="s">
+        <v>124</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="E8" s="70"/>
+      <c r="F8" s="143" t="s">
+        <v>125</v>
+      </c>
+      <c r="G8" s="122">
+        <f>M8</f>
+        <v>154736.84210526317</v>
+      </c>
+      <c r="H8" s="140"/>
+      <c r="I8" s="72"/>
+      <c r="J8" s="72"/>
+      <c r="K8" s="72"/>
+      <c r="L8" s="180">
+        <f>Notes!E44</f>
+        <v>164988.7302779865</v>
+      </c>
+      <c r="M8" s="180">
+        <f>Notes!E52</f>
+        <v>154736.84210526317</v>
+      </c>
+      <c r="N8" s="69"/>
+      <c r="O8" s="133" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B9" s="67"/>
+      <c r="C9" s="75"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="76"/>
+      <c r="G9" s="73"/>
+      <c r="H9" s="73"/>
+      <c r="I9" s="73"/>
+      <c r="J9" s="73"/>
+      <c r="K9" s="73"/>
+      <c r="L9" s="73"/>
+      <c r="M9" s="73"/>
+      <c r="N9" s="73"/>
+      <c r="O9" s="113"/>
+    </row>
+    <row r="10" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="67"/>
+      <c r="C10" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="30"/>
-    </row>
-    <row r="9" spans="2:11" ht="16" thickBot="1">
-      <c r="B9" s="67"/>
-      <c r="C9" s="78" t="s">
-        <v>114</v>
-      </c>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="129" t="s">
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="30"/>
+    </row>
+    <row r="11" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="67"/>
+      <c r="C11" s="78" t="s">
+        <v>113</v>
+      </c>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="128" t="s">
         <v>3</v>
       </c>
-      <c r="G9" s="123">
+      <c r="G11" s="122">
         <f>ROUND(0,0)</f>
         <v>0</v>
       </c>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="30"/>
-    </row>
-    <row r="10" spans="2:11" ht="16" thickBot="1">
-      <c r="B10" s="67"/>
-      <c r="C10" s="78" t="s">
-        <v>113</v>
-      </c>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="71" t="s">
+      <c r="H11" s="74"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="30"/>
+    </row>
+    <row r="12" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="67"/>
+      <c r="C12" s="78" t="s">
+        <v>112</v>
+      </c>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="G10" s="123">
+      <c r="G12" s="122">
         <f>ROUND(0,0)</f>
         <v>0</v>
       </c>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="30"/>
-    </row>
-    <row r="11" spans="2:11" ht="16" thickBot="1">
-      <c r="B11" s="67"/>
-      <c r="C11" s="78" t="s">
+      <c r="H12" s="74"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="30"/>
+    </row>
+    <row r="13" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="67"/>
+      <c r="C13" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="78"/>
-      <c r="E11" s="78"/>
-      <c r="F11" s="71" t="s">
+      <c r="D13" s="78"/>
+      <c r="E13" s="78"/>
+      <c r="F13" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="G11" s="123">
+      <c r="G13" s="122">
         <f>ROUND(15,0)</f>
         <v>15</v>
       </c>
-      <c r="H11" s="73"/>
-      <c r="I11" s="73"/>
-      <c r="J11" s="74"/>
-      <c r="K11" s="119"/>
-    </row>
-    <row r="12" spans="2:11">
-      <c r="B12" s="67"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="74"/>
-      <c r="K12" s="59"/>
-    </row>
-    <row r="13" spans="2:11" ht="16" thickBot="1">
-      <c r="B13" s="67"/>
-      <c r="C13" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="59"/>
-    </row>
-    <row r="14" spans="2:11" ht="16" thickBot="1">
+      <c r="H13" s="74"/>
+      <c r="I13" s="73"/>
+      <c r="J13" s="73"/>
+      <c r="K13" s="73"/>
+      <c r="L13" s="73"/>
+      <c r="M13" s="73"/>
+      <c r="N13" s="74"/>
+      <c r="O13" s="118"/>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B14" s="67"/>
-      <c r="C14" s="109" t="s">
-        <v>94</v>
-      </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="109" t="s">
-        <v>31</v>
-      </c>
-      <c r="G14" s="77">
-        <f>ROUND(G15*G6*1000,2)</f>
-        <v>13000</v>
-      </c>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="12"/>
       <c r="H14" s="12"/>
       <c r="I14" s="12"/>
-      <c r="J14" s="73"/>
-      <c r="K14" s="120"/>
-    </row>
-    <row r="15" spans="2:11" ht="16" thickBot="1">
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="74"/>
+      <c r="O14" s="59"/>
+    </row>
+    <row r="15" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="67"/>
-      <c r="C15" s="79" t="s">
+      <c r="C15" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="59"/>
+    </row>
+    <row r="16" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="67"/>
+      <c r="C16" s="108" t="s">
+        <v>93</v>
+      </c>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="108" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" s="77">
+        <f>Notes!E28</f>
+        <v>12746.4</v>
+      </c>
+      <c r="H16" s="141"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="73"/>
+      <c r="O16" s="119"/>
+    </row>
+    <row r="17" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="67"/>
+      <c r="C17" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="79"/>
-      <c r="E15" s="79"/>
-      <c r="F15" s="110" t="s">
+      <c r="D17" s="79"/>
+      <c r="E17" s="79"/>
+      <c r="F17" s="131" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" s="77">
+        <v>1300</v>
+      </c>
+      <c r="H17" s="141"/>
+      <c r="I17" s="73"/>
+      <c r="J17" s="73"/>
+      <c r="K17" s="73"/>
+      <c r="L17" s="73"/>
+      <c r="M17" s="73"/>
+      <c r="N17" s="73"/>
+      <c r="O17" s="123"/>
+    </row>
+    <row r="18" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="67"/>
+      <c r="C18" s="115" t="s">
+        <v>94</v>
+      </c>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="121" t="s">
+        <v>105</v>
+      </c>
+      <c r="G18" s="80">
+        <f>I18</f>
+        <v>100</v>
+      </c>
+      <c r="H18" s="141"/>
+      <c r="I18" s="139">
+        <v>100</v>
+      </c>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
+      <c r="N18" s="73"/>
+      <c r="O18" s="123"/>
+    </row>
+    <row r="19" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="67"/>
+      <c r="C19" s="108" t="s">
+        <v>95</v>
+      </c>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="110" t="s">
         <v>91</v>
       </c>
-      <c r="G15" s="77">
-        <v>1300</v>
-      </c>
-      <c r="H15" s="73"/>
-      <c r="I15" s="73"/>
-      <c r="J15" s="73"/>
-      <c r="K15" s="124"/>
-    </row>
-    <row r="16" spans="2:11" ht="16" thickBot="1">
-      <c r="B16" s="67"/>
-      <c r="C16" s="116" t="s">
-        <v>95</v>
-      </c>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="122" t="s">
-        <v>106</v>
-      </c>
-      <c r="G16" s="80">
-        <v>100</v>
-      </c>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="73"/>
-      <c r="K16" s="124"/>
-    </row>
-    <row r="17" spans="2:11" ht="16" thickBot="1">
-      <c r="B17" s="67"/>
-      <c r="C17" s="109" t="s">
+      <c r="G19" s="80"/>
+      <c r="H19" s="141"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="73"/>
+      <c r="O19" s="123"/>
+    </row>
+    <row r="20" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="67"/>
+      <c r="C20" s="115" t="s">
         <v>96</v>
       </c>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="111" t="s">
-        <v>92</v>
-      </c>
-      <c r="G17" s="80"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="73"/>
-      <c r="K17" s="124"/>
-    </row>
-    <row r="18" spans="2:11" ht="16" thickBot="1">
-      <c r="B18" s="67"/>
-      <c r="C18" s="116" t="s">
-        <v>97</v>
-      </c>
-      <c r="D18" s="82"/>
-      <c r="E18" s="82"/>
-      <c r="F18" s="71" t="s">
+      <c r="D20" s="82"/>
+      <c r="E20" s="82"/>
+      <c r="F20" s="71" t="s">
         <v>50</v>
       </c>
-      <c r="G18" s="77">
+      <c r="G20" s="77">
         <v>0</v>
       </c>
-      <c r="H18" s="73"/>
-      <c r="I18" s="73"/>
-      <c r="J18" s="73"/>
-      <c r="K18" s="120"/>
-    </row>
-    <row r="19" spans="2:11" ht="16" thickBot="1">
-      <c r="B19" s="67"/>
-      <c r="C19" s="109" t="s">
-        <v>97</v>
-      </c>
-      <c r="D19" s="81"/>
-      <c r="E19" s="81"/>
-      <c r="F19" s="110" t="s">
+      <c r="H20" s="141"/>
+      <c r="I20" s="73"/>
+      <c r="J20" s="73"/>
+      <c r="K20" s="73"/>
+      <c r="L20" s="73"/>
+      <c r="M20" s="73"/>
+      <c r="N20" s="73"/>
+      <c r="O20" s="119"/>
+    </row>
+    <row r="21" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="67"/>
+      <c r="C21" s="108" t="s">
+        <v>96</v>
+      </c>
+      <c r="D21" s="81"/>
+      <c r="E21" s="81"/>
+      <c r="F21" s="109" t="s">
         <v>90</v>
       </c>
-      <c r="G19" s="83">
+      <c r="G21" s="138">
         <v>0</v>
       </c>
-      <c r="H19" s="73"/>
-      <c r="I19" s="73"/>
-      <c r="J19" s="73"/>
-      <c r="K19" s="30"/>
+      <c r="H21" s="73"/>
+      <c r="I21" s="73"/>
+      <c r="J21" s="73"/>
+      <c r="K21" s="73"/>
+      <c r="L21" s="73"/>
+      <c r="M21" s="73"/>
+      <c r="N21" s="73"/>
+      <c r="O21" s="30"/>
+    </row>
+    <row r="22" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C22" s="62" t="str">
+        <f>Dashboard!C32</f>
+        <v>cost_of_installing</v>
+      </c>
+      <c r="G22" s="139">
+        <f>I22</f>
+        <v>1500</v>
+      </c>
+      <c r="I22" s="139">
+        <f>Notes!E25</f>
+        <v>1500</v>
+      </c>
+      <c r="J22" s="76"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3691,28 +4301,28 @@
   <sheetPr codeName="Sheet4" enableFormatConditionsCalculation="0">
     <tabColor theme="6" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="B1:K5"/>
+  <dimension ref="B1:K21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="33.125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="33.140625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.25" style="45" customWidth="1"/>
-    <col min="2" max="2" width="3.375" style="45" customWidth="1"/>
-    <col min="3" max="3" width="27.5" style="45" customWidth="1"/>
-    <col min="4" max="4" width="3.125" style="45" customWidth="1"/>
-    <col min="5" max="5" width="16.125" style="45" customWidth="1"/>
-    <col min="6" max="6" width="10.25" style="45" customWidth="1"/>
-    <col min="7" max="9" width="12.125" style="45" customWidth="1"/>
-    <col min="10" max="10" width="11.5" style="46" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" style="45" customWidth="1"/>
+    <col min="2" max="2" width="3.42578125" style="45" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" style="45" customWidth="1"/>
+    <col min="4" max="4" width="3.140625" style="45" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" style="45" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" style="45" customWidth="1"/>
+    <col min="7" max="9" width="12.140625" style="45" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" style="46" customWidth="1"/>
     <col min="11" max="11" width="66" style="45" customWidth="1"/>
-    <col min="12" max="16384" width="33.125" style="45"/>
+    <col min="12" max="16384" width="33.140625" style="45"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="16" thickBot="1"/>
-    <row r="2" spans="2:11">
+    <row r="1" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B2" s="47"/>
       <c r="C2" s="48"/>
       <c r="D2" s="48"/>
@@ -3722,9 +4332,9 @@
       <c r="H2" s="48"/>
       <c r="I2" s="48"/>
       <c r="J2" s="49"/>
-      <c r="K2" s="48"/>
-    </row>
-    <row r="3" spans="2:11">
+      <c r="K2" s="184"/>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B3" s="50"/>
       <c r="C3" s="51" t="s">
         <v>21</v>
@@ -3736,9 +4346,9 @@
       <c r="H3" s="51"/>
       <c r="I3" s="51"/>
       <c r="J3" s="52"/>
-      <c r="K3" s="53"/>
-    </row>
-    <row r="4" spans="2:11">
+      <c r="K3" s="185"/>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B4" s="50"/>
       <c r="C4" s="53"/>
       <c r="D4" s="53"/>
@@ -3748,9 +4358,9 @@
       <c r="H4" s="53"/>
       <c r="I4" s="53"/>
       <c r="J4" s="54"/>
-      <c r="K4" s="53"/>
-    </row>
-    <row r="5" spans="2:11">
+      <c r="K4" s="185"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B5" s="55"/>
       <c r="C5" s="56" t="s">
         <v>28</v>
@@ -3766,25 +4376,1174 @@
         <v>29</v>
       </c>
       <c r="H5" s="56" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I5" s="56" t="s">
         <v>58</v>
       </c>
       <c r="J5" s="57" t="s">
+        <v>115</v>
+      </c>
+      <c r="K5" s="186" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B6" s="50"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="185"/>
+    </row>
+    <row r="7" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="50"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="54"/>
+      <c r="K7" s="185"/>
+    </row>
+    <row r="8" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="50"/>
+      <c r="C8" s="132"/>
+      <c r="D8" s="132"/>
+      <c r="E8" s="132" t="s">
         <v>116</v>
       </c>
-      <c r="K5" s="56" t="s">
-        <v>15</v>
-      </c>
+      <c r="F8" s="132"/>
+      <c r="G8" s="132"/>
+      <c r="H8" s="132"/>
+      <c r="I8" s="132"/>
+      <c r="J8" s="125" t="s">
+        <v>52</v>
+      </c>
+      <c r="K8" s="134"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B9" s="50"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="53"/>
+      <c r="I9" s="53"/>
+      <c r="J9" s="54"/>
+      <c r="K9" s="185"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B10" s="50"/>
+      <c r="C10" s="135" t="str">
+        <f>Dashboard!C32</f>
+        <v>cost_of_installing</v>
+      </c>
+      <c r="D10" s="132"/>
+      <c r="E10" s="132" t="s">
+        <v>117</v>
+      </c>
+      <c r="F10" s="132" t="s">
+        <v>118</v>
+      </c>
+      <c r="G10" s="132"/>
+      <c r="H10" s="132"/>
+      <c r="I10" s="136">
+        <v>42948</v>
+      </c>
+      <c r="J10" s="137" t="s">
+        <v>119</v>
+      </c>
+      <c r="K10" s="134" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B11" s="50"/>
+      <c r="C11" s="137" t="str">
+        <f>Dashboard!C$13</f>
+        <v>storage.volume</v>
+      </c>
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="53"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="54"/>
+      <c r="K11" s="185"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B12" s="50"/>
+      <c r="C12" s="137"/>
+      <c r="D12" s="53"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="53"/>
+      <c r="I12" s="53"/>
+      <c r="J12" s="54"/>
+      <c r="K12" s="185"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B13" s="50"/>
+      <c r="C13" s="137" t="str">
+        <f>Dashboard!C13</f>
+        <v>storage.volume</v>
+      </c>
+      <c r="D13" s="132"/>
+      <c r="E13" s="132" t="s">
+        <v>126</v>
+      </c>
+      <c r="F13" s="132" t="s">
+        <v>118</v>
+      </c>
+      <c r="G13" s="132">
+        <v>2010</v>
+      </c>
+      <c r="H13" s="132" t="s">
+        <v>127</v>
+      </c>
+      <c r="I13" s="136">
+        <v>42948</v>
+      </c>
+      <c r="J13" s="146" t="s">
+        <v>128</v>
+      </c>
+      <c r="K13" s="134"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B14" s="50"/>
+      <c r="C14" s="137"/>
+      <c r="D14" s="132"/>
+      <c r="E14" s="132"/>
+      <c r="F14" s="132"/>
+      <c r="G14" s="132"/>
+      <c r="H14" s="132"/>
+      <c r="I14" s="136"/>
+      <c r="J14" s="146"/>
+      <c r="K14" s="134"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B15" s="50"/>
+      <c r="C15" s="137" t="str">
+        <f>Dashboard!C$13</f>
+        <v>storage.volume</v>
+      </c>
+      <c r="D15" s="132"/>
+      <c r="E15" s="132" t="s">
+        <v>129</v>
+      </c>
+      <c r="F15" s="132" t="s">
+        <v>118</v>
+      </c>
+      <c r="G15" s="132" t="s">
+        <v>127</v>
+      </c>
+      <c r="H15" s="132" t="s">
+        <v>127</v>
+      </c>
+      <c r="I15" s="136">
+        <v>42948</v>
+      </c>
+      <c r="J15" s="146" t="s">
+        <v>130</v>
+      </c>
+      <c r="K15" s="134"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B16" s="50"/>
+      <c r="C16" s="53"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="53"/>
+      <c r="G16" s="53"/>
+      <c r="H16" s="53"/>
+      <c r="I16" s="53"/>
+      <c r="J16" s="54"/>
+      <c r="K16" s="185"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B17" s="50"/>
+      <c r="C17" s="54" t="str">
+        <f>Dashboard!C$14</f>
+        <v>storage.cost_per_mwh</v>
+      </c>
+      <c r="D17" s="53"/>
+      <c r="E17" s="53" t="s">
+        <v>154</v>
+      </c>
+      <c r="F17" s="132" t="s">
+        <v>118</v>
+      </c>
+      <c r="G17" s="53" t="s">
+        <v>127</v>
+      </c>
+      <c r="H17" s="53" t="s">
+        <v>127</v>
+      </c>
+      <c r="I17" s="187">
+        <v>42979</v>
+      </c>
+      <c r="J17" s="188" t="s">
+        <v>153</v>
+      </c>
+      <c r="K17" s="185"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B18" s="50"/>
+      <c r="C18" s="53"/>
+      <c r="D18" s="53"/>
+      <c r="E18" s="53"/>
+      <c r="F18" s="53"/>
+      <c r="G18" s="53"/>
+      <c r="H18" s="53"/>
+      <c r="I18" s="53"/>
+      <c r="J18" s="54"/>
+      <c r="K18" s="185"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B19" s="50"/>
+      <c r="C19" s="54" t="str">
+        <f>Dashboard!C$14</f>
+        <v>storage.cost_per_mwh</v>
+      </c>
+      <c r="D19" s="53"/>
+      <c r="E19" s="53" t="s">
+        <v>158</v>
+      </c>
+      <c r="F19" s="132" t="s">
+        <v>118</v>
+      </c>
+      <c r="G19" s="53" t="s">
+        <v>127</v>
+      </c>
+      <c r="H19" s="53" t="s">
+        <v>127</v>
+      </c>
+      <c r="I19" s="187">
+        <v>42979</v>
+      </c>
+      <c r="J19" s="157" t="s">
+        <v>159</v>
+      </c>
+      <c r="K19" s="185"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B20" s="50"/>
+      <c r="C20" s="53"/>
+      <c r="D20" s="53"/>
+      <c r="E20" s="53"/>
+      <c r="F20" s="53"/>
+      <c r="G20" s="53"/>
+      <c r="H20" s="53"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="54"/>
+      <c r="K20" s="185"/>
+    </row>
+    <row r="21" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="189"/>
+      <c r="C21" s="190"/>
+      <c r="D21" s="190"/>
+      <c r="E21" s="190"/>
+      <c r="F21" s="190"/>
+      <c r="G21" s="190"/>
+      <c r="H21" s="190"/>
+      <c r="I21" s="190"/>
+      <c r="J21" s="191"/>
+      <c r="K21" s="192"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J17" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:J59"/>
+  <sheetViews>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:XFD59"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.5703125" style="147" customWidth="1"/>
+    <col min="2" max="2" width="4.140625" style="147" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" style="147" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.7109375" style="147" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" style="147" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.28515625" style="147" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" style="147" customWidth="1"/>
+    <col min="8" max="9" width="10.7109375" style="147"/>
+    <col min="10" max="10" width="136.28515625" style="147" customWidth="1"/>
+    <col min="11" max="16384" width="10.7109375" style="147"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B3" s="148"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="149"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B4" s="99"/>
+      <c r="C4" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="150"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B5" s="151"/>
+      <c r="C5" s="152"/>
+      <c r="D5" s="152"/>
+      <c r="E5" s="152"/>
+      <c r="F5" s="152"/>
+      <c r="G5" s="152"/>
+      <c r="H5" s="152"/>
+      <c r="I5" s="152"/>
+      <c r="J5" s="153"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B6" s="151"/>
+      <c r="C6" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="D6" s="52"/>
+      <c r="E6" s="152"/>
+      <c r="F6" s="152"/>
+      <c r="G6" s="152" t="s">
+        <v>132</v>
+      </c>
+      <c r="H6" s="152"/>
+      <c r="I6" s="152"/>
+      <c r="J6" s="153"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B7" s="151"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="152" t="s">
+        <v>133</v>
+      </c>
+      <c r="E7" s="154">
+        <v>10</v>
+      </c>
+      <c r="F7" s="154" t="s">
+        <v>134</v>
+      </c>
+      <c r="G7" s="152"/>
+      <c r="H7" s="152"/>
+      <c r="I7" s="152"/>
+      <c r="J7" s="153"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B8" s="151"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="152" t="s">
+        <v>135</v>
+      </c>
+      <c r="E8" s="154">
+        <v>10</v>
+      </c>
+      <c r="F8" s="154" t="s">
+        <v>136</v>
+      </c>
+      <c r="G8" s="152"/>
+      <c r="H8" s="152"/>
+      <c r="I8" s="152"/>
+      <c r="J8" s="153"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B9" s="151"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="152" t="s">
+        <v>137</v>
+      </c>
+      <c r="E9" s="154">
+        <v>4.18</v>
+      </c>
+      <c r="F9" s="154" t="s">
+        <v>138</v>
+      </c>
+      <c r="G9" s="152"/>
+      <c r="H9" s="152"/>
+      <c r="I9" s="152"/>
+      <c r="J9" s="153"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B10" s="151"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="152" t="s">
+        <v>139</v>
+      </c>
+      <c r="E10" s="154">
+        <v>10</v>
+      </c>
+      <c r="F10" s="154" t="s">
+        <v>140</v>
+      </c>
+      <c r="G10" s="152" t="s">
+        <v>141</v>
+      </c>
+      <c r="H10" s="152"/>
+      <c r="I10" s="152"/>
+      <c r="J10" s="153"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B11" s="151"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="152" t="s">
+        <v>142</v>
+      </c>
+      <c r="E11" s="155">
+        <f>E7*60*E8/E9/E10</f>
+        <v>143.54066985645935</v>
+      </c>
+      <c r="F11" s="154" t="s">
+        <v>143</v>
+      </c>
+      <c r="G11" s="152"/>
+      <c r="H11" s="152"/>
+      <c r="I11" s="152"/>
+      <c r="J11" s="153"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B12" s="151"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="152" t="s">
+        <v>144</v>
+      </c>
+      <c r="E12" s="155">
+        <v>3600000</v>
+      </c>
+      <c r="F12" s="154" t="s">
+        <v>145</v>
+      </c>
+      <c r="G12" s="152"/>
+      <c r="H12" s="152"/>
+      <c r="I12" s="152"/>
+      <c r="J12" s="153"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B13" s="151"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="156" t="str">
+        <f>Dashboard!C$13</f>
+        <v>storage.volume</v>
+      </c>
+      <c r="E13" s="154">
+        <f>MROUND(E11*E10*E9/E12,0.0001)</f>
+        <v>1.7000000000000001E-3</v>
+      </c>
+      <c r="F13" s="172" t="str">
+        <f>Dashboard!D$13</f>
+        <v>MWh</v>
+      </c>
+      <c r="G13" s="152"/>
+      <c r="H13" s="157"/>
+      <c r="I13" s="152"/>
+      <c r="J13" s="153"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B14" s="151"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="152"/>
+      <c r="E14" s="152"/>
+      <c r="F14" s="152"/>
+      <c r="G14" s="152"/>
+      <c r="H14" s="152"/>
+      <c r="I14" s="152"/>
+      <c r="J14" s="153"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B15" s="151"/>
+      <c r="C15" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="D15" s="152" t="s">
+        <v>133</v>
+      </c>
+      <c r="E15" s="154">
+        <v>20</v>
+      </c>
+      <c r="F15" s="154" t="s">
+        <v>134</v>
+      </c>
+      <c r="G15" s="152"/>
+      <c r="H15" s="152"/>
+      <c r="I15" s="152"/>
+      <c r="J15" s="153"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B16" s="151"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="152" t="s">
+        <v>135</v>
+      </c>
+      <c r="E16" s="154">
+        <v>10</v>
+      </c>
+      <c r="F16" s="154" t="s">
+        <v>136</v>
+      </c>
+      <c r="G16" s="152"/>
+      <c r="H16" s="152"/>
+      <c r="I16" s="152"/>
+      <c r="J16" s="153"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B17" s="151"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="152" t="s">
+        <v>137</v>
+      </c>
+      <c r="E17" s="154">
+        <v>4.18</v>
+      </c>
+      <c r="F17" s="154" t="s">
+        <v>138</v>
+      </c>
+      <c r="G17" s="152"/>
+      <c r="H17" s="152"/>
+      <c r="I17" s="152"/>
+      <c r="J17" s="153"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B18" s="151"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="152" t="s">
+        <v>139</v>
+      </c>
+      <c r="E18" s="154">
+        <v>10</v>
+      </c>
+      <c r="F18" s="154" t="s">
+        <v>140</v>
+      </c>
+      <c r="G18" s="152" t="s">
+        <v>141</v>
+      </c>
+      <c r="H18" s="152"/>
+      <c r="I18" s="152"/>
+      <c r="J18" s="153"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B19" s="151"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="152" t="s">
+        <v>142</v>
+      </c>
+      <c r="E19" s="155">
+        <f>E15*60*E16/E17/E18</f>
+        <v>287.08133971291869</v>
+      </c>
+      <c r="F19" s="154" t="s">
+        <v>143</v>
+      </c>
+      <c r="G19" s="152"/>
+      <c r="H19" s="152"/>
+      <c r="I19" s="152"/>
+      <c r="J19" s="153"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B20" s="151"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="152" t="s">
+        <v>144</v>
+      </c>
+      <c r="E20" s="155">
+        <v>3600000</v>
+      </c>
+      <c r="F20" s="154" t="s">
+        <v>145</v>
+      </c>
+      <c r="G20" s="152"/>
+      <c r="H20" s="152"/>
+      <c r="I20" s="152"/>
+      <c r="J20" s="153"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B21" s="151"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="156" t="str">
+        <f>Dashboard!C$13</f>
+        <v>storage.volume</v>
+      </c>
+      <c r="E21" s="154">
+        <f>MROUND(E19*E18*E17/E20,0.0001)</f>
+        <v>3.3E-3</v>
+      </c>
+      <c r="F21" s="172" t="str">
+        <f>Dashboard!D$13</f>
+        <v>MWh</v>
+      </c>
+      <c r="G21" s="152"/>
+      <c r="H21" s="152"/>
+      <c r="I21" s="152"/>
+      <c r="J21" s="153"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B22" s="151"/>
+      <c r="C22" s="152"/>
+      <c r="D22" s="152"/>
+      <c r="E22" s="152"/>
+      <c r="F22" s="152"/>
+      <c r="G22" s="152"/>
+      <c r="H22" s="152"/>
+      <c r="I22" s="152"/>
+      <c r="J22" s="153"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B23" s="151"/>
+      <c r="C23" s="152"/>
+      <c r="D23" s="152"/>
+      <c r="E23" s="152"/>
+      <c r="F23" s="152"/>
+      <c r="G23" s="152"/>
+      <c r="H23" s="152"/>
+      <c r="I23" s="152"/>
+      <c r="J23" s="153"/>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B24" s="151"/>
+      <c r="C24" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="D24" s="156" t="str">
+        <f>Dashboard!C$13</f>
+        <v>storage.volume</v>
+      </c>
+      <c r="E24" s="147">
+        <v>0</v>
+      </c>
+      <c r="F24" s="172" t="str">
+        <f>Dashboard!D$13</f>
+        <v>MWh</v>
+      </c>
+      <c r="G24" s="152" t="s">
+        <v>146</v>
+      </c>
+      <c r="H24" s="152"/>
+      <c r="I24" s="152"/>
+      <c r="J24" s="153"/>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B25" s="151"/>
+      <c r="C25" s="152"/>
+      <c r="D25" s="152" t="str">
+        <f>Dashboard!C32</f>
+        <v>cost_of_installing</v>
+      </c>
+      <c r="E25" s="152">
+        <v>1500</v>
+      </c>
+      <c r="F25" s="152" t="s">
+        <v>31</v>
+      </c>
+      <c r="G25" s="152"/>
+      <c r="H25" s="152"/>
+      <c r="I25" s="152"/>
+      <c r="J25" s="153"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B26" s="151"/>
+      <c r="C26" s="152"/>
+      <c r="D26" s="152" t="s">
+        <v>160</v>
+      </c>
+      <c r="E26" s="152">
+        <v>13000</v>
+      </c>
+      <c r="F26" s="152" t="s">
+        <v>31</v>
+      </c>
+      <c r="G26" s="152"/>
+      <c r="H26" s="152"/>
+      <c r="I26" s="152"/>
+      <c r="J26" s="153"/>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B27" s="151"/>
+      <c r="C27" s="152"/>
+      <c r="D27" s="152" t="s">
+        <v>161</v>
+      </c>
+      <c r="E27" s="181">
+        <v>253.6</v>
+      </c>
+      <c r="F27" s="152" t="s">
+        <v>31</v>
+      </c>
+      <c r="G27" s="152" t="s">
+        <v>162</v>
+      </c>
+      <c r="H27" s="152"/>
+      <c r="I27" s="152"/>
+      <c r="J27" s="153"/>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B28" s="151"/>
+      <c r="C28" s="152"/>
+      <c r="D28" s="182" t="str">
+        <f>Dashboard!C30</f>
+        <v>initial_investment</v>
+      </c>
+      <c r="E28" s="183">
+        <f>E26-E27</f>
+        <v>12746.4</v>
+      </c>
+      <c r="F28" s="152" t="s">
+        <v>31</v>
+      </c>
+      <c r="G28" s="152"/>
+      <c r="H28" s="152"/>
+      <c r="I28" s="152"/>
+      <c r="J28" s="153"/>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B29" s="151"/>
+      <c r="C29" s="152"/>
+      <c r="D29" s="152"/>
+      <c r="E29" s="152"/>
+      <c r="F29" s="152"/>
+      <c r="G29" s="152"/>
+      <c r="H29" s="152"/>
+      <c r="I29" s="152"/>
+      <c r="J29" s="153"/>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B30" s="151"/>
+      <c r="C30" s="152"/>
+      <c r="D30" s="152"/>
+      <c r="E30" s="152"/>
+      <c r="F30" s="152"/>
+      <c r="G30" s="152"/>
+      <c r="H30" s="152"/>
+      <c r="I30" s="152"/>
+      <c r="J30" s="153"/>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B31" s="151"/>
+      <c r="C31" s="152"/>
+      <c r="D31" s="152"/>
+      <c r="E31" s="152"/>
+      <c r="F31" s="152"/>
+      <c r="G31" s="152"/>
+      <c r="H31" s="152"/>
+      <c r="I31" s="152"/>
+      <c r="J31" s="153"/>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B32" s="151"/>
+      <c r="C32" s="152"/>
+      <c r="D32" s="152"/>
+      <c r="E32" s="152"/>
+      <c r="F32" s="152"/>
+      <c r="G32" s="152"/>
+      <c r="H32" s="152"/>
+      <c r="I32" s="152"/>
+      <c r="J32" s="153"/>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B33" s="151"/>
+      <c r="C33" s="178" t="s">
+        <v>154</v>
+      </c>
+      <c r="D33" s="178"/>
+      <c r="E33" s="152"/>
+      <c r="F33" s="152"/>
+      <c r="G33" s="152"/>
+      <c r="H33" s="152"/>
+      <c r="I33" s="152"/>
+      <c r="J33" s="153"/>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B34" s="151"/>
+      <c r="C34" s="152"/>
+      <c r="D34" s="152" t="s">
+        <v>148</v>
+      </c>
+      <c r="E34">
+        <v>4.18</v>
+      </c>
+      <c r="F34" t="s">
+        <v>138</v>
+      </c>
+      <c r="G34" s="152"/>
+      <c r="H34" s="152"/>
+      <c r="I34" s="152"/>
+      <c r="J34" s="153"/>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B35" s="151"/>
+      <c r="C35" s="152"/>
+      <c r="D35" s="152" t="s">
+        <v>147</v>
+      </c>
+      <c r="E35">
+        <v>10</v>
+      </c>
+      <c r="F35" t="s">
+        <v>140</v>
+      </c>
+      <c r="G35" s="152"/>
+      <c r="H35" s="152"/>
+      <c r="I35" s="152"/>
+      <c r="J35" s="153"/>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B36" s="151"/>
+      <c r="C36" s="152"/>
+      <c r="D36" s="152"/>
+      <c r="E36" s="152">
+        <f>E34*E35</f>
+        <v>41.8</v>
+      </c>
+      <c r="F36" s="152" t="s">
+        <v>149</v>
+      </c>
+      <c r="G36" s="152"/>
+      <c r="H36" s="152"/>
+      <c r="I36" s="152"/>
+      <c r="J36" s="153"/>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B37" s="151"/>
+      <c r="C37" s="152"/>
+      <c r="D37" s="152"/>
+      <c r="E37" s="152">
+        <v>3600000</v>
+      </c>
+      <c r="F37" s="152" t="s">
+        <v>150</v>
+      </c>
+      <c r="G37" s="152"/>
+      <c r="H37" s="152"/>
+      <c r="I37" s="152"/>
+      <c r="J37" s="153"/>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B38" s="151"/>
+      <c r="C38" s="152"/>
+      <c r="D38" s="152"/>
+      <c r="E38" s="174">
+        <f>E36/E37</f>
+        <v>1.161111111111111E-5</v>
+      </c>
+      <c r="F38" s="152" t="s">
+        <v>151</v>
+      </c>
+      <c r="G38" s="152"/>
+      <c r="H38" s="152"/>
+      <c r="I38" s="152"/>
+      <c r="J38" s="153"/>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B39" s="151"/>
+      <c r="C39" s="152"/>
+      <c r="D39" s="152"/>
+      <c r="E39" s="147">
+        <v>500</v>
+      </c>
+      <c r="F39" s="147" t="s">
+        <v>143</v>
+      </c>
+      <c r="G39" s="152"/>
+      <c r="H39" s="152"/>
+      <c r="I39" s="152"/>
+      <c r="J39" s="153"/>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B40" s="151"/>
+      <c r="C40" s="152"/>
+      <c r="D40" s="152" t="s">
+        <v>155</v>
+      </c>
+      <c r="E40" s="152">
+        <v>1159</v>
+      </c>
+      <c r="F40" s="147" t="s">
+        <v>31</v>
+      </c>
+      <c r="G40" s="152"/>
+      <c r="H40" s="152"/>
+      <c r="I40" s="152"/>
+      <c r="J40" s="153"/>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B41" s="151"/>
+      <c r="C41" s="152"/>
+      <c r="D41" s="152" t="s">
+        <v>156</v>
+      </c>
+      <c r="E41" s="175">
+        <f>E40/1.21</f>
+        <v>957.85123966942149</v>
+      </c>
+      <c r="F41" s="147" t="s">
+        <v>31</v>
+      </c>
+      <c r="G41" s="152"/>
+      <c r="H41" s="152"/>
+      <c r="I41" s="152"/>
+      <c r="J41" s="153"/>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B42" s="151"/>
+      <c r="C42" s="152"/>
+      <c r="D42" s="152" t="s">
+        <v>157</v>
+      </c>
+      <c r="E42" s="177">
+        <f>E41/E39</f>
+        <v>1.9157024793388431</v>
+      </c>
+      <c r="F42" s="147" t="s">
+        <v>152</v>
+      </c>
+      <c r="G42" s="152"/>
+      <c r="H42" s="152"/>
+      <c r="I42" s="152"/>
+      <c r="J42" s="153"/>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B43" s="151"/>
+      <c r="C43" s="152"/>
+      <c r="G43" s="152"/>
+      <c r="H43" s="152"/>
+      <c r="I43" s="152"/>
+      <c r="J43" s="153"/>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B44" s="151"/>
+      <c r="C44" s="152"/>
+      <c r="D44" s="156" t="str">
+        <f>Dashboard!C$14</f>
+        <v>storage.cost_per_mwh</v>
+      </c>
+      <c r="E44" s="176">
+        <f>E42/E38</f>
+        <v>164988.7302779865</v>
+      </c>
+      <c r="F44" s="152" t="s">
+        <v>125</v>
+      </c>
+      <c r="G44" s="152"/>
+      <c r="H44" s="152"/>
+      <c r="I44" s="152"/>
+      <c r="J44" s="153"/>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B45" s="151"/>
+      <c r="C45" s="152"/>
+      <c r="D45" s="156"/>
+      <c r="E45" s="157"/>
+      <c r="F45" s="152"/>
+      <c r="G45" s="152"/>
+      <c r="H45" s="152"/>
+      <c r="I45" s="152"/>
+      <c r="J45" s="153"/>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B46" s="151"/>
+      <c r="C46" s="152"/>
+      <c r="D46" s="156"/>
+      <c r="E46" s="157"/>
+      <c r="F46" s="152"/>
+      <c r="G46" s="152"/>
+      <c r="H46" s="152"/>
+      <c r="I46" s="152"/>
+      <c r="J46" s="153"/>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B47" s="151"/>
+      <c r="C47" s="152"/>
+      <c r="D47" s="156"/>
+      <c r="E47" s="157"/>
+      <c r="F47" s="152"/>
+      <c r="G47" s="152"/>
+      <c r="H47" s="152"/>
+      <c r="I47" s="152"/>
+      <c r="J47" s="153"/>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B48" s="151"/>
+      <c r="C48" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="D48" s="152"/>
+      <c r="E48" s="147">
+        <v>300</v>
+      </c>
+      <c r="F48" s="147" t="s">
+        <v>143</v>
+      </c>
+      <c r="G48" s="152"/>
+      <c r="H48" s="152"/>
+      <c r="I48" s="152"/>
+      <c r="J48" s="153"/>
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B49" s="151"/>
+      <c r="C49" s="152"/>
+      <c r="D49" s="152" t="s">
+        <v>156</v>
+      </c>
+      <c r="E49" s="175">
+        <v>539</v>
+      </c>
+      <c r="F49" s="147" t="s">
+        <v>31</v>
+      </c>
+      <c r="G49" s="152"/>
+      <c r="H49" s="152"/>
+      <c r="I49" s="152"/>
+      <c r="J49" s="153"/>
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B50" s="151"/>
+      <c r="C50" s="152"/>
+      <c r="D50" s="152" t="s">
+        <v>157</v>
+      </c>
+      <c r="E50" s="177">
+        <f>E49/E48</f>
+        <v>1.7966666666666666</v>
+      </c>
+      <c r="F50" s="147" t="s">
+        <v>152</v>
+      </c>
+      <c r="G50" s="152"/>
+      <c r="H50" s="152"/>
+      <c r="I50" s="152"/>
+      <c r="J50" s="153"/>
+    </row>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B51" s="151"/>
+      <c r="C51" s="152"/>
+      <c r="G51" s="152"/>
+      <c r="H51" s="152"/>
+      <c r="I51" s="152"/>
+      <c r="J51" s="153"/>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B52" s="151"/>
+      <c r="C52" s="152"/>
+      <c r="D52" s="156" t="str">
+        <f>Dashboard!C$14</f>
+        <v>storage.cost_per_mwh</v>
+      </c>
+      <c r="E52" s="176">
+        <f>E50/E38</f>
+        <v>154736.84210526317</v>
+      </c>
+      <c r="F52" s="152" t="s">
+        <v>125</v>
+      </c>
+      <c r="G52" s="152"/>
+      <c r="H52" s="152"/>
+      <c r="I52" s="152"/>
+      <c r="J52" s="153"/>
+    </row>
+    <row r="53" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B53" s="151"/>
+      <c r="C53" s="152"/>
+      <c r="G53" s="152"/>
+      <c r="H53" s="152"/>
+      <c r="I53" s="152"/>
+      <c r="J53" s="153"/>
+    </row>
+    <row r="54" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B54" s="151"/>
+      <c r="C54" s="152"/>
+      <c r="D54" s="156"/>
+      <c r="E54" s="157"/>
+      <c r="F54" s="152"/>
+      <c r="G54" s="152"/>
+      <c r="H54" s="152"/>
+      <c r="I54" s="152"/>
+      <c r="J54" s="153"/>
+    </row>
+    <row r="55" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B55" s="151"/>
+      <c r="C55" s="152"/>
+      <c r="D55" s="156"/>
+      <c r="E55" s="157"/>
+      <c r="F55" s="152"/>
+      <c r="G55" s="152"/>
+      <c r="H55" s="152"/>
+      <c r="I55" s="152"/>
+      <c r="J55" s="153"/>
+    </row>
+    <row r="56" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B56" s="151"/>
+      <c r="C56" s="152"/>
+      <c r="D56" s="156"/>
+      <c r="E56" s="157"/>
+      <c r="F56" s="152"/>
+      <c r="G56" s="152"/>
+      <c r="H56" s="152"/>
+      <c r="I56" s="152"/>
+      <c r="J56" s="153"/>
+    </row>
+    <row r="57" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B57" s="151"/>
+      <c r="C57" s="152"/>
+      <c r="D57" s="156"/>
+      <c r="E57" s="157"/>
+      <c r="F57" s="152"/>
+      <c r="G57" s="152"/>
+      <c r="H57" s="152"/>
+      <c r="I57" s="152"/>
+      <c r="J57" s="153"/>
+    </row>
+    <row r="58" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B58" s="151"/>
+      <c r="C58" s="14"/>
+      <c r="F58" s="157"/>
+      <c r="G58" s="152"/>
+      <c r="H58" s="152"/>
+      <c r="I58" s="152"/>
+      <c r="J58" s="153"/>
+    </row>
+    <row r="59" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="158"/>
+      <c r="C59" s="159"/>
+      <c r="D59" s="159"/>
+      <c r="E59" s="159"/>
+      <c r="F59" s="159"/>
+      <c r="G59" s="159"/>
+      <c r="H59" s="159"/>
+      <c r="I59" s="159"/>
+      <c r="J59" s="160"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>